<commit_message>
adding column bugs solved, readme updated
</commit_message>
<xml_diff>
--- a/src/main/resources/static/test.xlsx
+++ b/src/main/resources/static/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\apache-poi-examples\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB683DE-40E7-46F2-987A-451013CB1E7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6318CFA7-6CF0-415A-9ABB-DAD715DB7CEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>NAME</t>
   </si>
@@ -42,26 +42,17 @@
     <t>ADRESS</t>
   </si>
   <si>
-    <t>son1</t>
-  </si>
-  <si>
-    <t>SON1</t>
-  </si>
-  <si>
-    <t>son</t>
-  </si>
-  <si>
-    <t>son2</t>
-  </si>
-  <si>
-    <t>SON2</t>
+    <t>MERGED TEL &amp; CITY</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,8 +60,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,30 +84,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.499984740745262"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,28 +118,19 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B15" sqref="B15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,14 +422,14 @@
     <col min="2" max="2" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -461,56 +439,46 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="3" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="7"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>